<commit_message>
added data for MicroProfile
</commit_message>
<xml_diff>
--- a/Data/Features_Analysis.xlsx
+++ b/Data/Features_Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saile\OneDrive - Otto-Friedrich-Universität Bamberg\ms-framework-comparison\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\work\conferences\2020_ESSE\comparison\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7188AE88-52C9-448B-A5A9-A453262F8A35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB52C12-13F5-4421-83F3-1A9A6EC440AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="168">
   <si>
     <t>JAVA</t>
   </si>
@@ -599,13 +599,73 @@
   <si>
     <t>supported;
 provides a testing framework for unittest and pytest</t>
+  </si>
+  <si>
+    <t>MicroProfile</t>
+  </si>
+  <si>
+    <t>supported;
+MicroProfile Config specification;
+implemented with Apache Geronimo Config, WebSphere Liberty, Payara Server, Smallrye, microBean</t>
+  </si>
+  <si>
+    <t>supported;
+MicroProfile JWT; 
+implemented with Hammock, Wildfly, TomiTribe</t>
+  </si>
+  <si>
+    <t>not supported;
+but planned with sandbox project "reactive"</t>
+  </si>
+  <si>
+    <t>supported;
+MicroProfile OpenAPI for OpenAPI specifications</t>
+  </si>
+  <si>
+    <t>supported;
+with JAX-RS</t>
+  </si>
+  <si>
+    <t>not supported;
+but possible with Jakarta Messaging</t>
+  </si>
+  <si>
+    <t>not supported;
+but possible with Jakarta Persistence</t>
+  </si>
+  <si>
+    <t>MicroProfile Fault Tolerance; MicroProfile Health Check; MicroProfile Metrics; MicroProfile Open Tracing</t>
+  </si>
+  <si>
+    <t>supported;
+with MicroProfile Fault Tolerance</t>
+  </si>
+  <si>
+    <t>support for Health Checks;
+with MicroProfile Health</t>
+  </si>
+  <si>
+    <t>supported;
+with MicroProfile Metrics</t>
+  </si>
+  <si>
+    <t>supported;
+with MicroProfile Open Tracing for OpenTracing API</t>
+  </si>
+  <si>
+    <t>supported;
+depending on Application Server</t>
+  </si>
+  <si>
+    <t>supported;
+with MicroShed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -686,7 +746,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -709,11 +769,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -743,14 +840,23 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1134,58 +1240,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z32"/>
+  <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="39.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.77734375" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="43.44140625" customWidth="1"/>
-    <col min="6" max="6" width="45.21875" customWidth="1"/>
-    <col min="7" max="7" width="41.6640625" customWidth="1"/>
-    <col min="8" max="8" width="38" customWidth="1"/>
-    <col min="9" max="9" width="37.44140625" customWidth="1"/>
-    <col min="10" max="10" width="37.109375" customWidth="1"/>
-    <col min="11" max="11" width="42.109375" customWidth="1"/>
-    <col min="12" max="12" width="37" customWidth="1"/>
-    <col min="13" max="13" width="10.5546875" customWidth="1"/>
-    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="1025" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" customWidth="1"/>
+    <col min="6" max="6" width="45.28515625" customWidth="1"/>
+    <col min="7" max="8" width="41.7109375" customWidth="1"/>
+    <col min="9" max="9" width="38" customWidth="1"/>
+    <col min="10" max="10" width="37.42578125" customWidth="1"/>
+    <col min="11" max="11" width="37.140625" customWidth="1"/>
+    <col min="12" max="12" width="42.140625" customWidth="1"/>
+    <col min="13" max="13" width="37" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="1026" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="4" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:27" s="4" customFormat="1" ht="17.45" customHeight="1">
       <c r="A1" s="2"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="13" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="14"/>
+      <c r="K1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="14"/>
+      <c r="M1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="N1" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="14"/>
-      <c r="O1" s="1"/>
+      <c r="O1" s="15"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -1197,8 +1303,9 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="AA1" s="1"/>
+    </row>
+    <row r="2" spans="1:27" s="6" customFormat="1">
       <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
@@ -1221,25 +1328,27 @@
         <v>9</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="5"/>
+      <c r="N2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -1251,8 +1360,9 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="AA2" s="1"/>
+    </row>
+    <row r="3" spans="1:27" ht="15">
       <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
@@ -1266,11 +1376,12 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
       <c r="N3" s="7"/>
-    </row>
-    <row r="4" spans="1:26" ht="62.4" x14ac:dyDescent="0.4">
+      <c r="O3" s="7"/>
+    </row>
+    <row r="4" spans="1:27" ht="72">
       <c r="A4" s="12" t="s">
         <v>17</v>
       </c>
@@ -1293,24 +1404,27 @@
         <v>93</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>42</v>
+        <v>154</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M4" s="7"/>
+        <v>38</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="N4" s="7"/>
-    </row>
-    <row r="5" spans="1:26" ht="124.8" x14ac:dyDescent="0.4">
+      <c r="O4" s="7"/>
+    </row>
+    <row r="5" spans="1:27" ht="129">
       <c r="A5" s="12" t="s">
         <v>18</v>
       </c>
@@ -1333,25 +1447,28 @@
         <v>72</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>41</v>
       </c>
       <c r="J5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="M5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-    </row>
-    <row r="6" spans="1:26" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A6" s="15" t="s">
+      <c r="O5" s="7"/>
+    </row>
+    <row r="6" spans="1:27" ht="43.5">
+      <c r="A6" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1373,11 +1490,11 @@
         <v>75</v>
       </c>
       <c r="H6" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="J6" s="7" t="s">
         <v>42</v>
       </c>
@@ -1387,10 +1504,13 @@
       <c r="L6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="7"/>
+      <c r="M6" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="N6" s="7"/>
-    </row>
-    <row r="7" spans="1:26" ht="93.6" x14ac:dyDescent="0.4">
+      <c r="O6" s="7"/>
+    </row>
+    <row r="7" spans="1:27" ht="86.25">
       <c r="A7" s="12" t="s">
         <v>136</v>
       </c>
@@ -1413,24 +1533,27 @@
         <v>95</v>
       </c>
       <c r="H7" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="J7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="K7" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="L7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="M7" s="7"/>
       <c r="N7" s="7"/>
-    </row>
-    <row r="8" spans="1:26" ht="93.6" x14ac:dyDescent="0.4">
+      <c r="O7" s="7"/>
+    </row>
+    <row r="8" spans="1:27" ht="100.5">
       <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
@@ -1443,16 +1566,19 @@
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="O8" s="7"/>
+    </row>
+    <row r="9" spans="1:27" ht="15">
       <c r="A9" s="12" t="s">
         <v>130</v>
       </c>
@@ -1489,10 +1615,13 @@
       <c r="L9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M9" s="7"/>
+      <c r="M9" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="N9" s="7"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="O9" s="7"/>
+    </row>
+    <row r="10" spans="1:27" ht="15">
       <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
@@ -1507,10 +1636,11 @@
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
-      <c r="M10" s="7"/>
+      <c r="M10" s="8"/>
       <c r="N10" s="7"/>
-    </row>
-    <row r="11" spans="1:26" ht="78" x14ac:dyDescent="0.4">
+      <c r="O10" s="7"/>
+    </row>
+    <row r="11" spans="1:27" ht="72">
       <c r="A11" s="12" t="s">
         <v>131</v>
       </c>
@@ -1533,24 +1663,27 @@
         <v>76</v>
       </c>
       <c r="H11" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="J11" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="J11" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="K11" s="7" t="s">
         <v>42</v>
       </c>
       <c r="L11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M11" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="M11" s="7"/>
       <c r="N11" s="7"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="O11" s="7"/>
+    </row>
+    <row r="12" spans="1:27" ht="15">
       <c r="A12" s="11" t="s">
         <v>22</v>
       </c>
@@ -1567,8 +1700,9 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
-    </row>
-    <row r="13" spans="1:26" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="O12" s="7"/>
+    </row>
+    <row r="13" spans="1:27" ht="29.25">
       <c r="A13" s="12" t="s">
         <v>132</v>
       </c>
@@ -1591,24 +1725,27 @@
         <v>38</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>42</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="L13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M13" s="7"/>
+      <c r="M13" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="N13" s="7"/>
-    </row>
-    <row r="14" spans="1:26" ht="93.6" x14ac:dyDescent="0.4">
+      <c r="O13" s="7"/>
+    </row>
+    <row r="14" spans="1:27" ht="86.25">
       <c r="A14" s="12" t="s">
         <v>23</v>
       </c>
@@ -1631,24 +1768,27 @@
         <v>77</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="I14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="J14" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="K14" s="7" t="s">
         <v>38</v>
       </c>
       <c r="L14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M14" s="7"/>
+      <c r="M14" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="N14" s="7"/>
-    </row>
-    <row r="15" spans="1:26" ht="124.8" x14ac:dyDescent="0.4">
+      <c r="O14" s="7"/>
+    </row>
+    <row r="15" spans="1:27" ht="114.75">
       <c r="A15" s="12" t="s">
         <v>24</v>
       </c>
@@ -1671,24 +1811,27 @@
         <v>39</v>
       </c>
       <c r="H15" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="J15" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="K15" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="L15" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="L15" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="M15" s="7"/>
+      <c r="M15" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="N15" s="7"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="O15" s="7"/>
+    </row>
+    <row r="16" spans="1:27" ht="15">
       <c r="A16" s="12" t="s">
         <v>133</v>
       </c>
@@ -1705,8 +1848,9 @@
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
-    </row>
-    <row r="17" spans="1:14" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="O16" s="7"/>
+    </row>
+    <row r="17" spans="1:15" ht="29.25">
       <c r="A17" s="11" t="s">
         <v>25</v>
       </c>
@@ -1727,8 +1871,9 @@
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
-    </row>
-    <row r="18" spans="1:14" ht="109.2" x14ac:dyDescent="0.4">
+      <c r="O17" s="7"/>
+    </row>
+    <row r="18" spans="1:15" ht="100.5">
       <c r="A18" s="12" t="s">
         <v>26</v>
       </c>
@@ -1751,24 +1896,27 @@
         <v>78</v>
       </c>
       <c r="H18" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="J18" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>41</v>
       </c>
       <c r="L18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="M18" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="M18" s="7"/>
       <c r="N18" s="7"/>
-    </row>
-    <row r="19" spans="1:14" ht="124.8" x14ac:dyDescent="0.4">
+      <c r="O18" s="7"/>
+    </row>
+    <row r="19" spans="1:15" ht="114.75">
       <c r="A19" s="11" t="s">
         <v>27</v>
       </c>
@@ -1784,15 +1932,18 @@
       <c r="G19" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H19" s="7"/>
+      <c r="H19" s="7" t="s">
+        <v>161</v>
+      </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
-    </row>
-    <row r="20" spans="1:14" ht="46.8" x14ac:dyDescent="0.4">
+      <c r="O19" s="7"/>
+    </row>
+    <row r="20" spans="1:15" ht="57.75">
       <c r="A20" s="12" t="s">
         <v>28</v>
       </c>
@@ -1815,24 +1966,27 @@
         <v>38</v>
       </c>
       <c r="H20" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="I20" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I20" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="J20" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="L20" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L20" s="7" t="s">
+      <c r="M20" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="M20" s="7"/>
       <c r="N20" s="7"/>
-    </row>
-    <row r="21" spans="1:14" ht="78" x14ac:dyDescent="0.4">
+      <c r="O20" s="7"/>
+    </row>
+    <row r="21" spans="1:15" ht="72">
       <c r="A21" s="12" t="s">
         <v>29</v>
       </c>
@@ -1855,24 +2009,27 @@
         <v>38</v>
       </c>
       <c r="H21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="I21" s="7" t="s">
+      <c r="J21" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="K21" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="K21" s="7" t="s">
+      <c r="L21" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="L21" s="7" t="s">
+      <c r="M21" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="M21" s="7"/>
       <c r="N21" s="7"/>
-    </row>
-    <row r="22" spans="1:14" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="O21" s="7"/>
+    </row>
+    <row r="22" spans="1:15" ht="43.5">
       <c r="A22" s="12" t="s">
         <v>30</v>
       </c>
@@ -1895,7 +2052,7 @@
         <v>38</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>41</v>
+        <v>162</v>
       </c>
       <c r="I22" s="7" t="s">
         <v>41</v>
@@ -1907,12 +2064,15 @@
         <v>41</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M22" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="N22" s="7"/>
-    </row>
-    <row r="23" spans="1:14" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="O22" s="7"/>
+    </row>
+    <row r="23" spans="1:15" ht="29.25">
       <c r="A23" s="12" t="s">
         <v>31</v>
       </c>
@@ -1935,24 +2095,27 @@
         <v>38</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I23" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="J23" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="K23" s="7" t="s">
         <v>38</v>
       </c>
       <c r="L23" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M23" s="7"/>
+      <c r="M23" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="N23" s="7"/>
-    </row>
-    <row r="24" spans="1:14" ht="62.4" x14ac:dyDescent="0.4">
+      <c r="O23" s="7"/>
+    </row>
+    <row r="24" spans="1:15" ht="72">
       <c r="A24" s="12" t="s">
         <v>32</v>
       </c>
@@ -1975,24 +2138,27 @@
         <v>38</v>
       </c>
       <c r="H24" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I24" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I24" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="J24" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K24" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="K24" s="7" t="s">
+      <c r="L24" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="L24" s="7" t="s">
+      <c r="M24" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="M24" s="7"/>
       <c r="N24" s="7"/>
-    </row>
-    <row r="25" spans="1:14" ht="124.8" x14ac:dyDescent="0.4">
+      <c r="O24" s="7"/>
+    </row>
+    <row r="25" spans="1:15" ht="114.75">
       <c r="A25" s="12" t="s">
         <v>33</v>
       </c>
@@ -2015,24 +2181,27 @@
         <v>81</v>
       </c>
       <c r="H25" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="I25" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="J25" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="J25" s="7" t="s">
+      <c r="K25" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="L25" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="L25" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M25" s="7"/>
+      <c r="M25" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="N25" s="7"/>
-    </row>
-    <row r="26" spans="1:14" ht="59.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="O25" s="7"/>
+    </row>
+    <row r="26" spans="1:15" ht="59.45" customHeight="1">
       <c r="A26" s="12" t="s">
         <v>34</v>
       </c>
@@ -2055,24 +2224,27 @@
         <v>82</v>
       </c>
       <c r="H26" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="I26" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I26" s="7" t="s">
+      <c r="J26" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="J26" s="7" t="s">
+      <c r="K26" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="K26" s="7" t="s">
+      <c r="L26" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="L26" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M26" s="7"/>
+      <c r="M26" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="N26" s="7"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="O26" s="7"/>
+    </row>
+    <row r="27" spans="1:15" ht="15">
       <c r="A27" s="11" t="s">
         <v>35</v>
       </c>
@@ -2088,19 +2260,20 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="H27" s="7"/>
       <c r="I27" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J27" s="7"/>
+      <c r="J27" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
-    </row>
-    <row r="28" spans="1:14" ht="46.8" x14ac:dyDescent="0.4">
+      <c r="O27" s="7"/>
+    </row>
+    <row r="28" spans="1:15" ht="43.5">
       <c r="A28" s="12" t="s">
         <v>36</v>
       </c>
@@ -2123,24 +2296,27 @@
         <v>83</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>42</v>
+        <v>166</v>
       </c>
       <c r="I28" s="7" t="s">
         <v>42</v>
       </c>
       <c r="J28" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K28" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>123</v>
       </c>
       <c r="L28" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="M28" s="7"/>
+      <c r="M28" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="N28" s="7"/>
-    </row>
-    <row r="29" spans="1:14" ht="46.8" x14ac:dyDescent="0.4">
+      <c r="O28" s="7"/>
+    </row>
+    <row r="29" spans="1:15" ht="43.5">
       <c r="A29" s="12" t="s">
         <v>134</v>
       </c>
@@ -2163,13 +2339,13 @@
         <v>151</v>
       </c>
       <c r="H29" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I29" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="I29" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="J29" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>41</v>
@@ -2177,10 +2353,13 @@
       <c r="L29" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="M29" s="7"/>
+      <c r="M29" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="N29" s="7"/>
-    </row>
-    <row r="30" spans="1:14" ht="140.4" x14ac:dyDescent="0.4">
+      <c r="O29" s="7"/>
+    </row>
+    <row r="30" spans="1:15" ht="143.25">
       <c r="A30" s="12" t="s">
         <v>135</v>
       </c>
@@ -2209,7 +2388,7 @@
         <v>42</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>117</v>
+        <v>42</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>117</v>
@@ -2217,10 +2396,13 @@
       <c r="L30" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="M30" s="7"/>
+      <c r="M30" s="7" t="s">
+        <v>117</v>
+      </c>
       <c r="N30" s="7"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="O30" s="7"/>
+    </row>
+    <row r="31" spans="1:15" ht="15">
       <c r="A31" s="11" t="s">
         <v>37</v>
       </c>
@@ -2230,15 +2412,16 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="8"/>
+      <c r="H31" s="7"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
-      <c r="M31" s="7"/>
+      <c r="M31" s="8"/>
       <c r="N31" s="7"/>
-    </row>
-    <row r="32" spans="1:14" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="O31" s="7"/>
+    </row>
+    <row r="32" spans="1:15" ht="29.25">
       <c r="A32" s="12" t="s">
         <v>137</v>
       </c>
@@ -2275,15 +2458,18 @@
       <c r="L32" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M32" s="7"/>
+      <c r="M32" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="B1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added data for service coordination, now service workflows
</commit_message>
<xml_diff>
--- a/Data/Features_Analysis.xlsx
+++ b/Data/Features_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\work\conferences\2020_ESSE\comparison\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB52C12-13F5-4421-83F3-1A9A6EC440AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAE9B50-B9F0-44D9-9536-E942BC45BEA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="170">
   <si>
     <t>JAVA</t>
   </si>
@@ -526,9 +526,6 @@
     <t>4.1 API Gateway</t>
   </si>
   <si>
-    <t>4.4 Service Coordination</t>
-  </si>
-  <si>
     <t>7.2 Testing</t>
   </si>
   <si>
@@ -659,6 +656,17 @@
   <si>
     <t>supported;
 with MicroShed</t>
+  </si>
+  <si>
+    <t>supported;
+Support for the Saga Pattern</t>
+  </si>
+  <si>
+    <t>supported;
+Support for the Saga Pattern with Eventuate Tram Sagas</t>
+  </si>
+  <si>
+    <t>4.4 Service Workflows</t>
   </si>
 </sst>
 </file>
@@ -1243,8 +1251,8 @@
   <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H23" sqref="H23"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
@@ -1261,8 +1269,8 @@
     <col min="11" max="11" width="37.140625" customWidth="1"/>
     <col min="12" max="12" width="42.140625" customWidth="1"/>
     <col min="13" max="13" width="37" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" customWidth="1"/>
     <col min="16" max="1026" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1328,7 +1336,7 @@
         <v>9</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>10</v>
@@ -1404,7 +1412,7 @@
         <v>93</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>42</v>
@@ -1490,7 +1498,7 @@
         <v>75</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>41</v>
@@ -1512,7 +1520,7 @@
     </row>
     <row r="7" spans="1:27" ht="86.25">
       <c r="A7" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>42</v>
@@ -1521,7 +1529,7 @@
         <v>42</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>55</v>
@@ -1533,7 +1541,7 @@
         <v>95</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>86</v>
@@ -1645,7 +1653,7 @@
         <v>131</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>42</v>
@@ -1654,16 +1662,16 @@
         <v>49</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>76</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>87</v>
@@ -1768,7 +1776,7 @@
         <v>77</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>38</v>
@@ -1811,7 +1819,7 @@
         <v>39</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>41</v>
@@ -1831,24 +1839,52 @@
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
     </row>
-    <row r="16" spans="1:27" ht="15">
+    <row r="16" spans="1:27" ht="43.5">
       <c r="A16" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
+        <v>169</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17" spans="1:15" ht="29.25">
       <c r="A17" s="11" t="s">
@@ -1878,7 +1914,7 @@
         <v>26</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>41</v>
@@ -1887,7 +1923,7 @@
         <v>52</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>68</v>
@@ -1896,7 +1932,7 @@
         <v>78</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>88</v>
@@ -1933,7 +1969,7 @@
         <v>79</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -1966,7 +2002,7 @@
         <v>38</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>89</v>
@@ -2052,7 +2088,7 @@
         <v>38</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I22" s="7" t="s">
         <v>41</v>
@@ -2095,7 +2131,7 @@
         <v>38</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>42</v>
@@ -2138,7 +2174,7 @@
         <v>38</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I24" s="7" t="s">
         <v>91</v>
@@ -2181,7 +2217,7 @@
         <v>81</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I25" s="7" t="s">
         <v>92</v>
@@ -2224,7 +2260,7 @@
         <v>82</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I26" s="7" t="s">
         <v>91</v>
@@ -2281,7 +2317,7 @@
         <v>42</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>42</v>
@@ -2290,13 +2326,13 @@
         <v>61</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>83</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I28" s="7" t="s">
         <v>42</v>
@@ -2318,31 +2354,31 @@
     </row>
     <row r="29" spans="1:15" ht="43.5">
       <c r="A29" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="G29" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="H29" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I29" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>152</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>38</v>
@@ -2361,7 +2397,7 @@
     </row>
     <row r="30" spans="1:15" ht="143.25">
       <c r="A30" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>42</v>
@@ -2373,7 +2409,7 @@
         <v>42</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>71</v>
@@ -2423,22 +2459,22 @@
     </row>
     <row r="32" spans="1:15" ht="29.25">
       <c r="A32" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>142</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
added moleculer and sorted alphabetical
</commit_message>
<xml_diff>
--- a/Data/Features_Analysis.xlsx
+++ b/Data/Features_Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\work\conferences\2020_ESSE\comparison\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saile\OneDrive - Otto-Friedrich-Universität Bamberg\ms-framework-comparison\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAE9B50-B9F0-44D9-9536-E942BC45BEA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC04499-8DB7-43F8-AE91-4C0C01CBCA7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="183">
   <si>
     <t>JAVA</t>
   </si>
@@ -181,10 +181,6 @@
 tracing extension for OpenTracing available</t>
   </si>
   <si>
-    <t xml:space="preserve">supported;
-possibl with Kafka, ActiveMQ, RabbitMQ and Redis Streams </t>
-  </si>
-  <si>
     <t xml:space="preserve">
 GitHub with tools for the framework;
 Log Viewer: Commandline tool to view the content of event logs;
@@ -474,10 +470,6 @@
   </si>
   <si>
     <t>supported;
-has an integrated message broker interface for event-driven architectures, can be implemented with PubSub/Google PubSub or RPC/gRPC as well as plugins for NATS, Kafka, RabbitMQ, Redis, NSQ, SQS, stan and Stomp</t>
-  </si>
-  <si>
-    <t>supported;
 uses random hashed load balancing</t>
   </si>
   <si>
@@ -498,10 +490,6 @@
 does offer "SecurityUtils", but cannot be implemented</t>
   </si>
   <si>
-    <t>supported;
-possible to generate HTML files automatically by joliedoc; OpenAPI support is also available</t>
-  </si>
-  <si>
     <t xml:space="preserve">supported;
 mainly relational databases supported (e.g. PostgreSQL, MySQL, Apache Derby, SQLite) but support for MongoDB is also available </t>
   </si>
@@ -667,13 +655,77 @@
   </si>
   <si>
     <t>4.4 Service Workflows</t>
+  </si>
+  <si>
+    <t>supported;
+implemented with Moluculer Runner</t>
+  </si>
+  <si>
+    <t>supported;
+implemented with a built-in service discovery</t>
+  </si>
+  <si>
+    <t>supported;
+implemented by moleculer-web (the official API gateway service)</t>
+  </si>
+  <si>
+    <t>supported;
+supported by https://github.com/davidnussio/moleculer-cqrs</t>
+  </si>
+  <si>
+    <t>supported;
+moleculer-web-swagger supports swagger</t>
+  </si>
+  <si>
+    <t>supported;
+possible to generate HTML files automatically by joliedoc; OpenAPI support is also available</t>
+  </si>
+  <si>
+    <t>supported;
+implemented by moleculer-web</t>
+  </si>
+  <si>
+    <t>supported;
+supports NATS, Kafka and Redis</t>
+  </si>
+  <si>
+    <t>supported;
+has an integrated message broker interface for event-driven architectures, can be implemented with PubSub/Google PubSub or RPC/gRPC as well as plugins for NATS, Kafka, RabbitMQ, Redis, NSQ, SQS, stan and Stomp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supported;
+possible with Kafka, ActiveMQ, RabbitMQ and Redis Streams </t>
+  </si>
+  <si>
+    <t>supported;
+moleculer-db as adapter for CouchDB Nano, MongoDB, Mongoose (NoSQL) and Postgres, MySQL, SQLite, MSSQL (SQL)</t>
+  </si>
+  <si>
+    <t>supported;
+built-in solution</t>
+  </si>
+  <si>
+    <t>supported;
+built-in solution for Round Robin, Random strategy, CPU usage-based, Latency-based, Custom strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supported;
+implemented by moleculer-metrics, supports Zipkin, Jaeger and Prometheus </t>
+  </si>
+  <si>
+    <t>supported;
+supports Zipkin, Jaeger and Datadog</t>
+  </si>
+  <si>
+    <t>supported;
+supports Jest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -710,7 +762,7 @@
       <name val="CMU Serif"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -751,6 +803,12 @@
       <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor rgb="FFBFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -818,7 +876,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -865,6 +923,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1248,58 +1309,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA32"/>
+  <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" customWidth="1"/>
-    <col min="6" max="6" width="45.28515625" customWidth="1"/>
-    <col min="7" max="8" width="41.7109375" customWidth="1"/>
-    <col min="9" max="9" width="38" customWidth="1"/>
-    <col min="10" max="10" width="37.42578125" customWidth="1"/>
-    <col min="11" max="11" width="37.140625" customWidth="1"/>
-    <col min="12" max="12" width="42.140625" customWidth="1"/>
-    <col min="13" max="13" width="37" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" customWidth="1"/>
-    <col min="16" max="1026" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="39.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
+    <col min="7" max="7" width="43.44140625" customWidth="1"/>
+    <col min="8" max="8" width="45.33203125" customWidth="1"/>
+    <col min="9" max="10" width="41.6640625" customWidth="1"/>
+    <col min="11" max="11" width="37" customWidth="1"/>
+    <col min="12" max="12" width="27" customWidth="1"/>
+    <col min="13" max="13" width="32.21875" customWidth="1"/>
+    <col min="14" max="14" width="38" customWidth="1"/>
+    <col min="15" max="15" width="37.44140625" customWidth="1"/>
+    <col min="16" max="1024" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="4" customFormat="1" ht="17.45" customHeight="1">
+    <row r="1" spans="1:25" s="4" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2"/>
       <c r="B1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="14" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="15"/>
+      <c r="N1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="15"/>
+      <c r="O1" s="14"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -1310,52 +1371,50 @@
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-    </row>
-    <row r="2" spans="1:27" s="6" customFormat="1">
+    </row>
+    <row r="2" spans="1:25" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="I2" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -1367,10 +1426,8 @@
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-    </row>
-    <row r="3" spans="1:27" ht="15">
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
@@ -1383,13 +1440,13 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
     </row>
-    <row r="4" spans="1:27" ht="72">
+    <row r="4" spans="1:25" ht="78" x14ac:dyDescent="0.4">
       <c r="A4" s="12" t="s">
         <v>17</v>
       </c>
@@ -1397,90 +1454,94 @@
         <v>42</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>42</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>153</v>
+        <v>64</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="L4" s="19"/>
       <c r="M4" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-    </row>
-    <row r="5" spans="1:27" ht="129">
+        <v>167</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="124.8" x14ac:dyDescent="0.4">
       <c r="A5" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="E5" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>118</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="L5" s="19"/>
       <c r="M5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-    </row>
-    <row r="6" spans="1:27" ht="43.5">
+        <v>168</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="31.2" x14ac:dyDescent="0.4">
       <c r="A6" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>42</v>
@@ -1489,115 +1550,119 @@
         <v>38</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>155</v>
+        <v>38</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="L6" s="19"/>
       <c r="M6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-    </row>
-    <row r="7" spans="1:27" ht="86.25">
+      <c r="N6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="93.6" x14ac:dyDescent="0.4">
       <c r="A7" s="12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>137</v>
+        <v>42</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="K7" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>42</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="L7" s="19"/>
       <c r="M7" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-    </row>
-    <row r="8" spans="1:27" ht="100.5">
+        <v>169</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="93.6" x14ac:dyDescent="0.4">
       <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" s="7"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
       <c r="H8" s="7" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
+      <c r="L8" s="19"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
+      <c r="N8" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="O8" s="7"/>
     </row>
-    <row r="9" spans="1:27" ht="15">
+    <row r="9" spans="1:25" ht="62.4" x14ac:dyDescent="0.4">
       <c r="A9" s="12" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>38</v>
@@ -1606,7 +1671,7 @@
         <v>42</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>42</v>
@@ -1620,22 +1685,24 @@
       <c r="K9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="L9" s="19"/>
       <c r="M9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-    </row>
-    <row r="10" spans="1:27" ht="15">
+        <v>170</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -1643,55 +1710,57 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-    </row>
-    <row r="11" spans="1:27" ht="72">
+      <c r="L10" s="19"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+    </row>
+    <row r="11" spans="1:25" ht="62.4" x14ac:dyDescent="0.4">
       <c r="A11" s="12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>138</v>
+        <v>42</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>49</v>
+        <v>135</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>139</v>
+        <v>48</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>42</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="L11" s="19"/>
       <c r="M11" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-    </row>
-    <row r="12" spans="1:27" ht="15">
+        <v>171</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A12" s="11" t="s">
         <v>22</v>
       </c>
@@ -1705,26 +1774,26 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
+      <c r="L12" s="19"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
     </row>
-    <row r="13" spans="1:27" ht="29.25">
+    <row r="13" spans="1:25" ht="31.2" x14ac:dyDescent="0.4">
       <c r="A13" s="12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>38</v>
@@ -1733,127 +1802,133 @@
         <v>38</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>38</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="L13" s="19"/>
       <c r="M13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-    </row>
-    <row r="14" spans="1:27" ht="86.25">
+        <v>173</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="93.6" x14ac:dyDescent="0.4">
       <c r="A14" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>157</v>
+        <v>38</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>38</v>
+        <v>154</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L14" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="L14" s="19"/>
       <c r="M14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-    </row>
-    <row r="15" spans="1:27" ht="114.75">
+        <v>173</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="109.2" x14ac:dyDescent="0.4">
       <c r="A15" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>46</v>
+        <v>175</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>56</v>
+        <v>176</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="G15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="J15" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>104</v>
-      </c>
       <c r="K15" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>119</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="L15" s="19"/>
       <c r="M15" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-    </row>
-    <row r="16" spans="1:27" ht="43.5">
+        <v>174</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="46.8" x14ac:dyDescent="0.4">
       <c r="A16" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>167</v>
+        <v>41</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>168</v>
+        <v>41</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>41</v>
+        <v>164</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>41</v>
+        <v>165</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>41</v>
@@ -1873,7 +1948,7 @@
       <c r="K16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L16" s="7" t="s">
+      <c r="L16" s="19" t="s">
         <v>41</v>
       </c>
       <c r="M16" s="7" t="s">
@@ -1886,229 +1961,237 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="29.25">
+    <row r="17" spans="1:15" ht="31.2" x14ac:dyDescent="0.4">
       <c r="A17" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="7" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
+      <c r="L17" s="19"/>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
     </row>
-    <row r="18" spans="1:15" ht="100.5">
+    <row r="18" spans="1:15" ht="109.2" x14ac:dyDescent="0.4">
       <c r="A18" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>142</v>
+        <v>41</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>52</v>
+        <v>139</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>143</v>
+        <v>41</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>159</v>
+        <v>67</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>88</v>
+        <v>156</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="L18" s="19"/>
       <c r="M18" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-    </row>
-    <row r="19" spans="1:15" ht="114.75">
+        <v>177</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="124.8" x14ac:dyDescent="0.4">
       <c r="A19" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="7"/>
-      <c r="C19" s="7" t="s">
-        <v>47</v>
-      </c>
+      <c r="C19" s="7"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="7" t="s">
+      <c r="E19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H19" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
+      <c r="I19" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
+      <c r="L19" s="19"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
     </row>
-    <row r="20" spans="1:15" ht="57.75">
+    <row r="20" spans="1:15" ht="46.8" x14ac:dyDescent="0.4">
       <c r="A20" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>98</v>
-      </c>
       <c r="E20" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>38</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>161</v>
+        <v>38</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>89</v>
+        <v>158</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>121</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="L20" s="19"/>
       <c r="M20" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-    </row>
-    <row r="21" spans="1:15" ht="72">
+        <v>178</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="78" x14ac:dyDescent="0.4">
       <c r="A21" s="12" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>57</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>106</v>
+        <v>38</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>120</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="L21" s="19"/>
       <c r="M21" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-    </row>
-    <row r="22" spans="1:15" ht="43.5">
+        <v>179</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="31.2" x14ac:dyDescent="0.4">
       <c r="A22" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>98</v>
-      </c>
       <c r="E22" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>38</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>161</v>
+        <v>38</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>41</v>
+        <v>158</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="L22" s="19"/>
       <c r="M22" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-    </row>
-    <row r="23" spans="1:15" ht="29.25">
+        <v>38</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="31.2" x14ac:dyDescent="0.4">
       <c r="A23" s="12" t="s">
         <v>31</v>
       </c>
@@ -2119,368 +2202,382 @@
         <v>38</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>38</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>161</v>
+        <v>38</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>107</v>
+        <v>158</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L23" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="L23" s="19"/>
       <c r="M23" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-    </row>
-    <row r="24" spans="1:15" ht="72">
+      <c r="N23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="62.4" x14ac:dyDescent="0.4">
       <c r="A24" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>162</v>
+        <v>38</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>91</v>
+        <v>159</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="L24" s="7" t="s">
-        <v>122</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="L24" s="19"/>
       <c r="M24" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-    </row>
-    <row r="25" spans="1:15" ht="114.75">
+        <v>180</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="124.8" x14ac:dyDescent="0.4">
       <c r="A25" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="H25" s="7" t="s">
-        <v>163</v>
+        <v>73</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>108</v>
+        <v>160</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="L25" s="7" t="s">
-        <v>40</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="L25" s="19"/>
       <c r="M25" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-    </row>
-    <row r="26" spans="1:15" ht="59.45" customHeight="1">
+        <v>180</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="O25" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="59.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="E26" s="7" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>164</v>
+        <v>69</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="L26" s="7" t="s">
-        <v>40</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="L26" s="19"/>
       <c r="M26" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-    </row>
-    <row r="27" spans="1:15" ht="15">
+        <v>181</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="E27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
-      <c r="I27" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
       <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
+      <c r="L27" s="19"/>
       <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-    </row>
-    <row r="28" spans="1:15" ht="43.5">
+      <c r="N27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="46.8" x14ac:dyDescent="0.4">
       <c r="A28" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="C28" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="L28" s="19"/>
+      <c r="M28" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O28" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="46.8" x14ac:dyDescent="0.4">
+      <c r="A29" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F28" s="7" t="s">
+      <c r="E29" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="H29" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="I29" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L29" s="19"/>
+      <c r="M29" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="140.4" x14ac:dyDescent="0.4">
+      <c r="A30" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J30" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="H28" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="L28" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="M28" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-    </row>
-    <row r="29" spans="1:15" ht="43.5">
-      <c r="A29" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-    </row>
-    <row r="30" spans="1:15" ht="143.25">
-      <c r="A30" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="K30" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="L30" s="7" t="s">
-        <v>117</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="L30" s="19"/>
       <c r="M30" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-    </row>
-    <row r="31" spans="1:15" ht="15">
+        <v>116</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
       <c r="F31" s="8"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
       <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-    </row>
-    <row r="32" spans="1:15" ht="29.25">
+      <c r="L31" s="19"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+    </row>
+    <row r="32" spans="1:15" ht="31.2" x14ac:dyDescent="0.4">
       <c r="A32" s="12" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>140</v>
+        <v>42</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>42</v>
+        <v>137</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>42</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>42</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>42</v>
+        <v>138</v>
       </c>
       <c r="I32" s="7" t="s">
         <v>42</v>
@@ -2491,21 +2588,23 @@
       <c r="K32" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L32" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="L32" s="19"/>
       <c r="M32" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O32" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
     <mergeCell ref="N1:O1"/>
-    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added data for devis
</commit_message>
<xml_diff>
--- a/Data/Features_Analysis.xlsx
+++ b/Data/Features_Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saile\OneDrive - Otto-Friedrich-Universität Bamberg\ms-framework-comparison\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\work\conferences\2020_ESSE\comparison\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC04499-8DB7-43F8-AE91-4C0C01CBCA7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34411037-C92F-46A4-8C45-E60B617A6AEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="184">
   <si>
     <t>JAVA</t>
   </si>
@@ -719,13 +719,17 @@
   <si>
     <t>supported;
 supports Jest</t>
+  </si>
+  <si>
+    <t>not supported;
+possible via PM2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -762,7 +766,7 @@
       <name val="CMU Serif"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -803,12 +807,6 @@
       <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor rgb="FFBFBFBF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -924,7 +922,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1311,31 +1309,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="39.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.109375" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
-    <col min="7" max="7" width="43.44140625" customWidth="1"/>
-    <col min="8" max="8" width="45.33203125" customWidth="1"/>
-    <col min="9" max="10" width="41.6640625" customWidth="1"/>
+    <col min="7" max="7" width="43.42578125" customWidth="1"/>
+    <col min="8" max="8" width="45.28515625" customWidth="1"/>
+    <col min="9" max="10" width="41.7109375" customWidth="1"/>
     <col min="11" max="11" width="37" customWidth="1"/>
     <col min="12" max="12" width="27" customWidth="1"/>
-    <col min="13" max="13" width="32.21875" customWidth="1"/>
+    <col min="13" max="13" width="32.28515625" customWidth="1"/>
     <col min="14" max="14" width="38" customWidth="1"/>
-    <col min="15" max="15" width="37.44140625" customWidth="1"/>
-    <col min="16" max="1024" width="10.5546875" customWidth="1"/>
+    <col min="15" max="15" width="37.42578125" customWidth="1"/>
+    <col min="16" max="1024" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:25" s="4" customFormat="1" ht="17.45" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="16" t="s">
         <v>2</v>
@@ -1372,7 +1370,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
-    <row r="2" spans="1:25" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:25" s="6" customFormat="1">
       <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
@@ -1427,7 +1425,7 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:25" ht="15">
       <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
@@ -1446,7 +1444,7 @@
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
     </row>
-    <row r="4" spans="1:25" ht="78" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:25" ht="72">
       <c r="A4" s="12" t="s">
         <v>17</v>
       </c>
@@ -1480,7 +1478,9 @@
       <c r="K4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="19"/>
+      <c r="L4" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M4" s="7" t="s">
         <v>167</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="124.8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:25" ht="129">
       <c r="A5" s="12" t="s">
         <v>18</v>
       </c>
@@ -1525,7 +1525,9 @@
       <c r="K5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L5" s="19"/>
+      <c r="L5" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M5" s="7" t="s">
         <v>168</v>
       </c>
@@ -1536,7 +1538,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="31.2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:25" ht="43.5">
       <c r="A6" s="13" t="s">
         <v>19</v>
       </c>
@@ -1570,7 +1572,9 @@
       <c r="K6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="19"/>
+      <c r="L6" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="M6" s="7" t="s">
         <v>42</v>
       </c>
@@ -1581,7 +1585,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="93.6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:25" ht="86.25">
       <c r="A7" s="12" t="s">
         <v>132</v>
       </c>
@@ -1615,7 +1619,9 @@
       <c r="K7" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="L7" s="19"/>
+      <c r="L7" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M7" s="7" t="s">
         <v>169</v>
       </c>
@@ -1626,7 +1632,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="93.6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:25" ht="100.5">
       <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
@@ -1651,7 +1657,7 @@
       </c>
       <c r="O8" s="7"/>
     </row>
-    <row r="9" spans="1:25" ht="62.4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:25" ht="57.75">
       <c r="A9" s="12" t="s">
         <v>127</v>
       </c>
@@ -1685,7 +1691,9 @@
       <c r="K9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="19"/>
+      <c r="L9" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M9" s="7" t="s">
         <v>170</v>
       </c>
@@ -1696,7 +1704,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:25" ht="15">
       <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
@@ -1715,7 +1723,7 @@
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
     </row>
-    <row r="11" spans="1:25" ht="62.4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:25" ht="57.75">
       <c r="A11" s="12" t="s">
         <v>128</v>
       </c>
@@ -1749,7 +1757,9 @@
       <c r="K11" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="L11" s="19"/>
+      <c r="L11" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M11" s="7" t="s">
         <v>171</v>
       </c>
@@ -1760,7 +1770,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:25" ht="15">
       <c r="A12" s="11" t="s">
         <v>22</v>
       </c>
@@ -1779,7 +1789,7 @@
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
     </row>
-    <row r="13" spans="1:25" ht="31.2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:25" ht="29.25">
       <c r="A13" s="12" t="s">
         <v>129</v>
       </c>
@@ -1813,7 +1823,9 @@
       <c r="K13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L13" s="19"/>
+      <c r="L13" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M13" s="7" t="s">
         <v>173</v>
       </c>
@@ -1824,7 +1836,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="93.6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:25" ht="86.25">
       <c r="A14" s="12" t="s">
         <v>23</v>
       </c>
@@ -1858,7 +1870,9 @@
       <c r="K14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L14" s="19"/>
+      <c r="L14" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M14" s="7" t="s">
         <v>173</v>
       </c>
@@ -1869,7 +1883,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="109.2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:25" ht="100.5">
       <c r="A15" s="12" t="s">
         <v>24</v>
       </c>
@@ -1903,7 +1917,9 @@
       <c r="K15" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L15" s="19"/>
+      <c r="L15" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M15" s="7" t="s">
         <v>174</v>
       </c>
@@ -1914,7 +1930,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:25" ht="43.5">
       <c r="A16" s="12" t="s">
         <v>166</v>
       </c>
@@ -1948,7 +1964,7 @@
       <c r="K16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L16" s="19" t="s">
+      <c r="L16" s="7" t="s">
         <v>41</v>
       </c>
       <c r="M16" s="7" t="s">
@@ -1961,7 +1977,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="31.2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" ht="29.25">
       <c r="A17" s="11" t="s">
         <v>25</v>
       </c>
@@ -1984,7 +2000,7 @@
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
     </row>
-    <row r="18" spans="1:15" ht="109.2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" ht="100.5">
       <c r="A18" s="12" t="s">
         <v>26</v>
       </c>
@@ -2018,7 +2034,9 @@
       <c r="K18" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="L18" s="19"/>
+      <c r="L18" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M18" s="7" t="s">
         <v>177</v>
       </c>
@@ -2029,7 +2047,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="124.8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" ht="114.75">
       <c r="A19" s="11" t="s">
         <v>27</v>
       </c>
@@ -2056,7 +2074,7 @@
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
     </row>
-    <row r="20" spans="1:15" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" ht="57.75">
       <c r="A20" s="12" t="s">
         <v>28</v>
       </c>
@@ -2090,7 +2108,9 @@
       <c r="K20" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="L20" s="19"/>
+      <c r="L20" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M20" s="7" t="s">
         <v>178</v>
       </c>
@@ -2101,7 +2121,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="78" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" ht="72">
       <c r="A21" s="12" t="s">
         <v>29</v>
       </c>
@@ -2135,7 +2155,9 @@
       <c r="K21" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="L21" s="19"/>
+      <c r="L21" s="7" t="s">
+        <v>183</v>
+      </c>
       <c r="M21" s="7" t="s">
         <v>179</v>
       </c>
@@ -2146,7 +2168,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="31.2" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" ht="43.5">
       <c r="A22" s="12" t="s">
         <v>30</v>
       </c>
@@ -2180,7 +2202,9 @@
       <c r="K22" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L22" s="19"/>
+      <c r="L22" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M22" s="7" t="s">
         <v>38</v>
       </c>
@@ -2191,7 +2215,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="31.2" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" ht="29.25">
       <c r="A23" s="12" t="s">
         <v>31</v>
       </c>
@@ -2225,7 +2249,9 @@
       <c r="K23" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L23" s="19"/>
+      <c r="L23" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M23" s="7" t="s">
         <v>38</v>
       </c>
@@ -2236,7 +2262,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="62.4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" ht="72">
       <c r="A24" s="12" t="s">
         <v>32</v>
       </c>
@@ -2270,7 +2296,9 @@
       <c r="K24" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="L24" s="19"/>
+      <c r="L24" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M24" s="7" t="s">
         <v>180</v>
       </c>
@@ -2281,7 +2309,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="124.8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" ht="114.75">
       <c r="A25" s="12" t="s">
         <v>33</v>
       </c>
@@ -2315,7 +2343,9 @@
       <c r="K25" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L25" s="19"/>
+      <c r="L25" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M25" s="7" t="s">
         <v>180</v>
       </c>
@@ -2326,7 +2356,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="59.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" ht="59.45" customHeight="1">
       <c r="A26" s="12" t="s">
         <v>34</v>
       </c>
@@ -2360,7 +2390,9 @@
       <c r="K26" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L26" s="19"/>
+      <c r="L26" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M26" s="7" t="s">
         <v>181</v>
       </c>
@@ -2371,7 +2403,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" ht="15">
       <c r="A27" s="11" t="s">
         <v>35</v>
       </c>
@@ -2400,7 +2432,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" ht="43.5">
       <c r="A28" s="12" t="s">
         <v>36</v>
       </c>
@@ -2434,7 +2466,9 @@
       <c r="K28" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L28" s="19"/>
+      <c r="L28" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="M28" s="7" t="s">
         <v>121</v>
       </c>
@@ -2445,7 +2479,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" ht="43.5">
       <c r="A29" s="12" t="s">
         <v>130</v>
       </c>
@@ -2479,7 +2513,9 @@
       <c r="K29" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L29" s="19"/>
+      <c r="L29" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M29" s="7" t="s">
         <v>182</v>
       </c>
@@ -2490,7 +2526,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="140.4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" ht="143.25">
       <c r="A30" s="12" t="s">
         <v>131</v>
       </c>
@@ -2524,7 +2560,9 @@
       <c r="K30" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="L30" s="19"/>
+      <c r="L30" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M30" s="7" t="s">
         <v>116</v>
       </c>
@@ -2535,7 +2573,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" ht="15">
       <c r="A31" s="11" t="s">
         <v>37</v>
       </c>
@@ -2554,7 +2592,7 @@
       <c r="N31" s="8"/>
       <c r="O31" s="8"/>
     </row>
-    <row r="32" spans="1:15" ht="31.2" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" ht="29.25">
       <c r="A32" s="12" t="s">
         <v>133</v>
       </c>
@@ -2588,7 +2626,9 @@
       <c r="K32" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L32" s="19"/>
+      <c r="L32" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="M32" s="7" t="s">
         <v>41</v>
       </c>

</xml_diff>